<commit_message>
Added data to new presentation
</commit_message>
<xml_diff>
--- a/presentations/tables.xlsx
+++ b/presentations/tables.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresp/Documents/R Projects/Trading bloque/presentations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0927E4A-9076-2442-8D05-6DB97BB3A59A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E2622F-7C57-FC42-B235-B721183DD212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="520" yWindow="460" windowWidth="27740" windowHeight="17020" activeTab="1" xr2:uid="{6D854A5A-DFA4-0F42-8C56-FA3756197850}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="520" yWindow="460" windowWidth="27740" windowHeight="17020" activeTab="2" xr2:uid="{6D854A5A-DFA4-0F42-8C56-FA3756197850}"/>
   </bookViews>
   <sheets>
     <sheet name="AQR" sheetId="1" r:id="rId1"/>
     <sheet name="pros-cons" sheetId="2" r:id="rId2"/>
+    <sheet name="fondos_seleccionados" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Portfolio</t>
   </si>
@@ -93,9 +94,6 @@
     <t>Institucionales</t>
   </si>
   <si>
-    <t>Se mueven menos</t>
-  </si>
-  <si>
     <t>A veces 'se quedan atrás'</t>
   </si>
   <si>
@@ -109,6 +107,42 @@
   </si>
   <si>
     <t>No siempre son puros</t>
+  </si>
+  <si>
+    <t>Menor divergencia</t>
+  </si>
+  <si>
+    <t>Fund</t>
+  </si>
+  <si>
+    <t>AUM</t>
+  </si>
+  <si>
+    <t>Dunn</t>
+  </si>
+  <si>
+    <t>Cheaspeake</t>
+  </si>
+  <si>
+    <t>Mulvaney</t>
+  </si>
+  <si>
+    <t>Crabel</t>
+  </si>
+  <si>
+    <t>Lynx</t>
+  </si>
+  <si>
+    <t>Transtrend</t>
+  </si>
+  <si>
+    <t>Management Fee</t>
+  </si>
+  <si>
+    <t>Performance Fee</t>
+  </si>
+  <si>
+    <t>Inicio</t>
   </si>
 </sst>
 </file>
@@ -118,7 +152,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -133,16 +167,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFD5EA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE9EBF5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -150,17 +214,95 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -618,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D72653E-8310-1643-857D-FB37DE22EB53}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,32 +818,172 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8320AED8-0D4B-D04F-B314-6BC117FA2ABE}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="76" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="7">
+        <v>663</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="51" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="10">
+        <v>170</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="E3" s="10">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="51" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="10">
+        <v>4582</v>
+      </c>
+      <c r="C4" s="15">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="E4" s="10">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="51" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="13">
+        <v>222</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="13">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="13">
+        <v>6361</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="13">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="26" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="10">
+        <v>1500</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0</v>
+      </c>
+      <c r="E7" s="10">
+        <v>2014</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E7">
+    <sortCondition ref="E2:E7"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Better MAR ranking table
</commit_message>
<xml_diff>
--- a/presentations/tables.xlsx
+++ b/presentations/tables.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresp/Documents/R Projects/Trading bloque/presentations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C049EB-6F47-BE4F-B5DD-ED7D3E63D52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FD8CE7-6BF0-BA4A-8B2D-B556F3E34455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="520" yWindow="460" windowWidth="27740" windowHeight="17020" xr2:uid="{6D854A5A-DFA4-0F42-8C56-FA3756197850}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="520" yWindow="460" windowWidth="27740" windowHeight="17020" activeTab="1" xr2:uid="{6D854A5A-DFA4-0F42-8C56-FA3756197850}"/>
   </bookViews>
   <sheets>
     <sheet name="AQR" sheetId="1" r:id="rId1"/>
-    <sheet name="pros-cons" sheetId="2" r:id="rId2"/>
-    <sheet name="fondos_seleccionados" sheetId="3" r:id="rId3"/>
+    <sheet name="MAR_Ranking" sheetId="4" r:id="rId2"/>
+    <sheet name="pros-cons" sheetId="2" r:id="rId3"/>
+    <sheet name="fondos_seleccionados" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>Portfolio</t>
   </si>
@@ -143,6 +144,81 @@
   </si>
   <si>
     <t>Inicio</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Chesapeake</t>
+  </si>
+  <si>
+    <t>Eckhardt</t>
+  </si>
+  <si>
+    <t>Estlander Alpha Trend</t>
+  </si>
+  <si>
+    <t>Estlander Freedom</t>
+  </si>
+  <si>
+    <t>Fort Global Contrarian</t>
+  </si>
+  <si>
+    <t>Fort Global Diversified</t>
+  </si>
+  <si>
+    <t>Fort Global Trend</t>
+  </si>
+  <si>
+    <t>Hamer Trading</t>
+  </si>
+  <si>
+    <t>Man AHL Alpha</t>
+  </si>
+  <si>
+    <t>Man AHL Evolution</t>
+  </si>
+  <si>
+    <t>Merit</t>
+  </si>
+  <si>
+    <t>Millburn</t>
+  </si>
+  <si>
+    <t>MSR Investments</t>
+  </si>
+  <si>
+    <t>Quicksilver</t>
+  </si>
+  <si>
+    <t>Rotella Capita</t>
+  </si>
+  <si>
+    <t>Salus Alpha Capital</t>
+  </si>
+  <si>
+    <t>SSARIS Diversified</t>
+  </si>
+  <si>
+    <t>SSARIS Securitized Note</t>
+  </si>
+  <si>
+    <t>SSARIS Global Multi-Strategy</t>
+  </si>
+  <si>
+    <t>Sunrise Capital</t>
+  </si>
+  <si>
+    <t>Transtrend Enhanced</t>
+  </si>
+  <si>
+    <t>Transtrend Standard</t>
+  </si>
+  <si>
+    <t>WG Wealth Guardian</t>
+  </si>
+  <si>
+    <t>Winton Futures Fund</t>
   </si>
 </sst>
 </file>
@@ -152,7 +228,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -178,6 +254,12 @@
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Roboto Condensed"/>
     </font>
   </fonts>
   <fills count="5">
@@ -264,7 +346,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -303,6 +385,11 @@
     <xf numFmtId="10" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -669,7 +756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC6FC87-CA82-DF43-BC32-A8B78CBFDC2E}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="207" workbookViewId="0">
+    <sheetView zoomScale="207" workbookViewId="0">
       <selection activeCell="E4" sqref="B4:E4"/>
     </sheetView>
   </sheetViews>
@@ -757,6 +844,1006 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D289E21-6D5D-2B4B-AC84-A6F7CCFE27FC}">
+  <dimension ref="A1:W26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="16">
+        <v>2000</v>
+      </c>
+      <c r="C1" s="16">
+        <f>B1+1</f>
+        <v>2001</v>
+      </c>
+      <c r="D1" s="16">
+        <f t="shared" ref="D1:W1" si="0">C1+1</f>
+        <v>2002</v>
+      </c>
+      <c r="E1" s="16">
+        <f t="shared" si="0"/>
+        <v>2003</v>
+      </c>
+      <c r="F1" s="16">
+        <f t="shared" si="0"/>
+        <v>2004</v>
+      </c>
+      <c r="G1" s="16">
+        <f t="shared" si="0"/>
+        <v>2005</v>
+      </c>
+      <c r="H1" s="16">
+        <f t="shared" si="0"/>
+        <v>2006</v>
+      </c>
+      <c r="I1" s="16">
+        <f t="shared" si="0"/>
+        <v>2007</v>
+      </c>
+      <c r="J1" s="16">
+        <f t="shared" si="0"/>
+        <v>2008</v>
+      </c>
+      <c r="K1" s="16">
+        <f t="shared" si="0"/>
+        <v>2009</v>
+      </c>
+      <c r="L1" s="16">
+        <f t="shared" si="0"/>
+        <v>2010</v>
+      </c>
+      <c r="M1" s="16">
+        <f t="shared" si="0"/>
+        <v>2011</v>
+      </c>
+      <c r="N1" s="16">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="O1" s="16">
+        <f t="shared" si="0"/>
+        <v>2013</v>
+      </c>
+      <c r="P1" s="16">
+        <f t="shared" si="0"/>
+        <v>2014</v>
+      </c>
+      <c r="Q1" s="16">
+        <f t="shared" si="0"/>
+        <v>2015</v>
+      </c>
+      <c r="R1" s="16">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="S1" s="16">
+        <f t="shared" si="0"/>
+        <v>2017</v>
+      </c>
+      <c r="T1" s="16">
+        <f t="shared" si="0"/>
+        <v>2018</v>
+      </c>
+      <c r="U1" s="16">
+        <f t="shared" si="0"/>
+        <v>2019</v>
+      </c>
+      <c r="V1" s="16">
+        <f t="shared" si="0"/>
+        <v>2020</v>
+      </c>
+      <c r="W1" s="16">
+        <f t="shared" si="0"/>
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="16">
+        <v>5</v>
+      </c>
+      <c r="C2" s="16">
+        <v>4</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16">
+        <v>5</v>
+      </c>
+      <c r="H2" s="16">
+        <v>4</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16">
+        <v>5</v>
+      </c>
+      <c r="E3" s="16">
+        <v>4</v>
+      </c>
+      <c r="F3" s="16">
+        <v>4</v>
+      </c>
+      <c r="G3" s="16">
+        <v>4</v>
+      </c>
+      <c r="H3" s="16">
+        <v>3</v>
+      </c>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16">
+        <v>4</v>
+      </c>
+      <c r="J4" s="16">
+        <v>4</v>
+      </c>
+      <c r="K4" s="16">
+        <v>2</v>
+      </c>
+      <c r="L4" s="16">
+        <v>3</v>
+      </c>
+      <c r="M4" s="16">
+        <v>3</v>
+      </c>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16">
+        <v>5</v>
+      </c>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16">
+        <v>3</v>
+      </c>
+      <c r="R7" s="16">
+        <v>1</v>
+      </c>
+      <c r="S7" s="16">
+        <v>1</v>
+      </c>
+      <c r="T7" s="16">
+        <v>2</v>
+      </c>
+      <c r="U7" s="16">
+        <v>3</v>
+      </c>
+      <c r="V7" s="16">
+        <v>2</v>
+      </c>
+      <c r="W7" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16">
+        <v>5</v>
+      </c>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16">
+        <v>5</v>
+      </c>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16">
+        <v>5</v>
+      </c>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16">
+        <v>4</v>
+      </c>
+      <c r="V8" s="16">
+        <v>4</v>
+      </c>
+      <c r="W8" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="16">
+        <v>3</v>
+      </c>
+      <c r="C9" s="16">
+        <v>5</v>
+      </c>
+      <c r="D9" s="16">
+        <v>4</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="16"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16">
+        <v>4</v>
+      </c>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="16"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16">
+        <v>1</v>
+      </c>
+      <c r="N11" s="16">
+        <v>1</v>
+      </c>
+      <c r="O11" s="16">
+        <v>1</v>
+      </c>
+      <c r="P11" s="16">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="16">
+        <v>2</v>
+      </c>
+      <c r="R11" s="16">
+        <v>3</v>
+      </c>
+      <c r="S11" s="16">
+        <v>2</v>
+      </c>
+      <c r="T11" s="16">
+        <v>3</v>
+      </c>
+      <c r="U11" s="16">
+        <v>5</v>
+      </c>
+      <c r="V11" s="16">
+        <v>5</v>
+      </c>
+      <c r="W11" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="16"/>
+      <c r="V13" s="16"/>
+      <c r="W13" s="16"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="16">
+        <v>4</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16">
+        <v>5</v>
+      </c>
+      <c r="F14" s="16">
+        <v>5</v>
+      </c>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="16"/>
+      <c r="W14" s="16"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="16">
+        <v>2</v>
+      </c>
+      <c r="C15" s="16">
+        <v>2</v>
+      </c>
+      <c r="D15" s="16">
+        <v>2</v>
+      </c>
+      <c r="E15" s="16">
+        <v>2</v>
+      </c>
+      <c r="F15" s="16">
+        <v>2</v>
+      </c>
+      <c r="G15" s="16">
+        <v>2</v>
+      </c>
+      <c r="H15" s="16">
+        <v>2</v>
+      </c>
+      <c r="I15" s="16">
+        <v>3</v>
+      </c>
+      <c r="J15" s="16">
+        <v>5</v>
+      </c>
+      <c r="K15" s="16">
+        <v>3</v>
+      </c>
+      <c r="L15" s="16">
+        <v>2</v>
+      </c>
+      <c r="M15" s="16">
+        <v>2</v>
+      </c>
+      <c r="N15" s="16">
+        <v>2</v>
+      </c>
+      <c r="O15" s="16">
+        <v>2</v>
+      </c>
+      <c r="P15" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="16">
+        <v>1</v>
+      </c>
+      <c r="R15" s="16">
+        <v>2</v>
+      </c>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="16"/>
+      <c r="W15" s="16"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16">
+        <v>5</v>
+      </c>
+      <c r="N16" s="16">
+        <v>4</v>
+      </c>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="16"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16">
+        <v>2</v>
+      </c>
+      <c r="J17" s="16">
+        <v>3</v>
+      </c>
+      <c r="K17" s="16">
+        <v>4</v>
+      </c>
+      <c r="L17" s="16">
+        <v>5</v>
+      </c>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+      <c r="W17" s="16"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="16">
+        <v>2</v>
+      </c>
+      <c r="V18" s="16">
+        <v>3</v>
+      </c>
+      <c r="W18" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16">
+        <v>3</v>
+      </c>
+      <c r="D19" s="16">
+        <v>3</v>
+      </c>
+      <c r="E19" s="16">
+        <v>3</v>
+      </c>
+      <c r="F19" s="16">
+        <v>3</v>
+      </c>
+      <c r="G19" s="16">
+        <v>3</v>
+      </c>
+      <c r="H19" s="16">
+        <v>5</v>
+      </c>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="16"/>
+      <c r="V19" s="16"/>
+      <c r="W19" s="16"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A20" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="16">
+        <v>1</v>
+      </c>
+      <c r="C20" s="16">
+        <v>1</v>
+      </c>
+      <c r="D20" s="16">
+        <v>1</v>
+      </c>
+      <c r="E20" s="16">
+        <v>1</v>
+      </c>
+      <c r="F20" s="16">
+        <v>1</v>
+      </c>
+      <c r="G20" s="16">
+        <v>1</v>
+      </c>
+      <c r="H20" s="16">
+        <v>1</v>
+      </c>
+      <c r="I20" s="16">
+        <v>1</v>
+      </c>
+      <c r="J20" s="16">
+        <v>1</v>
+      </c>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
+      <c r="V20" s="16"/>
+      <c r="W20" s="16"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A21" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16">
+        <v>4</v>
+      </c>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
+      <c r="T21" s="16"/>
+      <c r="U21" s="16"/>
+      <c r="V21" s="16"/>
+      <c r="W21" s="16"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A22" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16">
+        <v>5</v>
+      </c>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
+      <c r="T22" s="16"/>
+      <c r="U22" s="16"/>
+      <c r="V22" s="16"/>
+      <c r="W22" s="16"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A23" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16">
+        <v>4</v>
+      </c>
+      <c r="N23" s="16">
+        <v>3</v>
+      </c>
+      <c r="O23" s="16">
+        <v>4</v>
+      </c>
+      <c r="P23" s="16">
+        <v>4</v>
+      </c>
+      <c r="Q23" s="16">
+        <v>4</v>
+      </c>
+      <c r="R23" s="16">
+        <v>5</v>
+      </c>
+      <c r="S23" s="16">
+        <v>4</v>
+      </c>
+      <c r="T23" s="16">
+        <v>5</v>
+      </c>
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
+      <c r="W23" s="16"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16">
+        <v>2</v>
+      </c>
+      <c r="K24" s="16">
+        <v>1</v>
+      </c>
+      <c r="L24" s="16">
+        <v>1</v>
+      </c>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16">
+        <v>5</v>
+      </c>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="16"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="16"/>
+      <c r="V24" s="16"/>
+      <c r="W24" s="16"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16">
+        <v>3</v>
+      </c>
+      <c r="P25" s="16">
+        <v>3</v>
+      </c>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="16"/>
+      <c r="V25" s="16"/>
+      <c r="W25" s="16"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A26" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16">
+        <v>3</v>
+      </c>
+      <c r="T26" s="16">
+        <v>1</v>
+      </c>
+      <c r="U26" s="16">
+        <v>1</v>
+      </c>
+      <c r="V26" s="16">
+        <v>1</v>
+      </c>
+      <c r="W26" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D72653E-8310-1643-857D-FB37DE22EB53}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -848,7 +1935,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8320AED8-0D4B-D04F-B314-6BC117FA2ABE}">
   <dimension ref="A1:E7"/>
   <sheetViews>

</xml_diff>